<commit_message>
documentation in a seperate file. only my own exceptions explained
</commit_message>
<xml_diff>
--- a/Timetable/Lipovits.xlsx
+++ b/Timetable/Lipovits.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -50,20 +50,38 @@
   <si>
     <t>12 new, seperate diagrams</t>
   </si>
+  <si>
+    <t>loadtesting</t>
+  </si>
+  <si>
+    <t>read property file</t>
+  </si>
+  <si>
+    <t>Loadtesting + man. Client</t>
+  </si>
+  <si>
+    <t>Exceptions, create Clients</t>
+  </si>
+  <si>
+    <t>man. Client</t>
+  </si>
+  <si>
+    <t>Commands Prototype</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY" numFmtId="166"/>
-    <numFmt formatCode="HH:MM" numFmtId="167"/>
+    <numFmt formatCode="DD/MM/YYYY" numFmtId="165"/>
+    <numFmt formatCode="HH:MM" numFmtId="166"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -90,10 +108,17 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
@@ -168,7 +193,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -177,35 +202,39 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -229,7 +258,7 @@
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="F6" activeCellId="0" pane="topLeft" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -302,48 +331,84 @@
           <t/>
         </is>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
+      <c r="A4" s="6" t="n">
+        <v>41675</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
         <f aca="false">C4-B4</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5">
+      <c r="A5" s="6" t="n">
+        <v>41679</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
         <f aca="false">C5-B5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
+      <c r="A6" s="6" t="n">
+        <v>41681</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.555555555555556</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.597222222222222</v>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
         <f aca="false">C6-B6</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
@@ -1561,7 +1626,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="atEnd" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>